<commit_message>
Added excel files for the APA analysis
These excel files contain the parameters for the activity detection
</commit_message>
<xml_diff>
--- a/First iteration/data/excel files/ES39.xlsx
+++ b/First iteration/data/excel files/ES39.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="49">
   <si>
     <t>Filename</t>
   </si>
@@ -131,6 +131,36 @@
   </si>
   <si>
     <t>Datei enthält 12 Gangepisoden, Kompassspur irgendwie komisch</t>
+  </si>
+  <si>
+    <t>LTSD Parameters</t>
+  </si>
+  <si>
+    <t>Right</t>
+  </si>
+  <si>
+    <t>Left</t>
+  </si>
+  <si>
+    <t>Win</t>
+  </si>
+  <si>
+    <t>Threshols</t>
+  </si>
+  <si>
+    <t>Threshold</t>
+  </si>
+  <si>
+    <t>200.0</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>100.0</t>
+  </si>
+  <si>
+    <t>5.0</t>
   </si>
 </sst>
 </file>
@@ -962,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K16"/>
+  <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:AG17"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -979,7 +1009,7 @@
     <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -993,7 +1023,7 @@
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -1019,10 +1049,35 @@
         <v>30</v>
       </c>
       <c r="K2" t="s">
+        <v>39</v>
+      </c>
+      <c r="O2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+      <c r="M3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>42</v>
+      </c>
+      <c r="M4" t="s">
+        <v>44</v>
+      </c>
+      <c r="N4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -1048,10 +1103,22 @@
         <v>3.6342593E-3</v>
       </c>
       <c r="K5" t="s">
+        <v>46</v>
+      </c>
+      <c r="L5" t="s">
+        <v>47</v>
+      </c>
+      <c r="M5" t="s">
+        <v>48</v>
+      </c>
+      <c r="N5" t="s">
+        <v>45</v>
+      </c>
+      <c r="O5" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1059,7 +1126,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1067,7 +1134,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1075,7 +1142,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>10</v>
       </c>
@@ -1083,7 +1150,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -1091,7 +1158,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1099,7 +1166,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>16</v>
       </c>
@@ -1107,7 +1174,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>18</v>
       </c>
@@ -1115,7 +1182,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>20</v>
       </c>
@@ -1123,7 +1190,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>22</v>
       </c>
@@ -1131,7 +1198,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>24</v>
       </c>

</xml_diff>